<commit_message>
Added analysis for the 07/11
</commit_message>
<xml_diff>
--- a/data/channels.xlsx
+++ b/data/channels.xlsx
@@ -8,19 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\quotaclimat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A91F56-2C39-49C3-B232-A00C478F05C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832F955F-9737-498F-A7B9-3CDA4AE4B036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14055" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping" sheetId="2" r:id="rId1"/>
     <sheet name="top_audiences" sheetId="3" r:id="rId2"/>
-    <sheet name="top_audiences (2)" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">mapping!$A$1:$D$683</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">top_audiences!$A$1:$B$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'top_audiences (2)'!$A$1:$C$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="1321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="1324">
   <si>
     <t>lci</t>
   </si>
@@ -4006,6 +4004,15 @@
   </si>
   <si>
     <t>Radio</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Généraliste</t>
+  </si>
+  <si>
+    <t>Information en continu</t>
   </si>
 </sst>
 </file>
@@ -10126,9 +10133,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7143151D-8E71-411B-A1BA-2A4686C6EBB2}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -10137,7 +10144,7 @@
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1315</v>
       </c>
@@ -10147,8 +10154,11 @@
       <c r="C1" t="s">
         <v>1317</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -10158,8 +10168,11 @@
       <c r="C2" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -10169,8 +10182,11 @@
       <c r="C3" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -10180,8 +10196,11 @@
       <c r="C4" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
@@ -10191,8 +10210,11 @@
       <c r="C5" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -10202,8 +10224,11 @@
       <c r="C6" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -10213,8 +10238,11 @@
       <c r="C7" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>201</v>
       </c>
@@ -10224,8 +10252,11 @@
       <c r="C8" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>219</v>
       </c>
@@ -10235,8 +10266,11 @@
       <c r="C9" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>209</v>
       </c>
@@ -10246,8 +10280,11 @@
       <c r="C10" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>205</v>
       </c>
@@ -10257,8 +10294,11 @@
       <c r="C11" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>217</v>
       </c>
@@ -10268,16 +10308,22 @@
       <c r="C12" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C13" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>1235</v>
       </c>
@@ -10287,8 +10333,11 @@
       <c r="C14" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -10298,8 +10347,11 @@
       <c r="C15" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
@@ -10309,8 +10361,11 @@
       <c r="C16" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>223</v>
       </c>
@@ -10320,8 +10375,11 @@
       <c r="C17" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>242</v>
       </c>
@@ -10331,8 +10389,11 @@
       <c r="C18" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>258</v>
       </c>
@@ -10342,8 +10403,11 @@
       <c r="C19" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>228</v>
       </c>
@@ -10353,8 +10417,11 @@
       <c r="C20" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>230</v>
       </c>
@@ -10364,8 +10431,11 @@
       <c r="C21" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>232</v>
       </c>
@@ -10375,8 +10445,11 @@
       <c r="C22" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>234</v>
       </c>
@@ -10386,8 +10459,11 @@
       <c r="C23" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
@@ -10397,24 +10473,33 @@
       <c r="C24" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C25" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>748</v>
       </c>
       <c r="C26" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>45</v>
       </c>
@@ -10422,7 +10507,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
@@ -10433,7 +10518,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>47</v>
       </c>
@@ -10444,7 +10529,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -10455,7 +10540,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>49</v>
       </c>
@@ -10466,7 +10551,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>195</v>
       </c>
@@ -10638,531 +10723,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ACE5FC3-2409-49E9-A66A-F0DB0A69BA25}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:C51"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>1315</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1316</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1317</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2">
-        <v>19.7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>14.7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>9.4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>9.1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6">
-        <v>3.3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8">
-        <v>2.9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B9">
-        <v>2.6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B10">
-        <v>2.5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="B13">
-        <v>1.9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B14">
-        <v>1.6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B15">
-        <v>1.5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="B16">
-        <v>1.5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B17">
-        <v>1.5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B18">
-        <v>1.2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B19">
-        <v>1.2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B20">
-        <v>1.2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>1235</v>
-      </c>
-      <c r="B23">
-        <v>0.8</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>748</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28">
-        <v>31.6</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29">
-        <v>24</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30">
-        <v>18.3</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31">
-        <v>15.7</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B32">
-        <v>11</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B33">
-        <v>6.2</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="B34">
-        <v>5.7</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C38" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
-        <v>767</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>1246</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>769</v>
-      </c>
-      <c r="C44" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
-        <v>783</v>
-      </c>
-      <c r="C45" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C46" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>773</v>
-      </c>
-      <c r="C47" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>954</v>
-      </c>
-      <c r="C49" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>775</v>
-      </c>
-      <c r="C50" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>1264</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:C51" xr:uid="{4ACE5FC3-2409-49E9-A66A-F0DB0A69BA25}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="TV"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C26">
-      <sortCondition descending="1" ref="B1:B51"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>